<commit_message>
Add Streamlit app link
</commit_message>
<xml_diff>
--- a/results/scenarios/scenarios_summary_gurobi_20250711_1007.xlsx
+++ b/results/scenarios/scenarios_summary_gurobi_20250711_1007.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqgchal2\Documents\pypsa\results\high-level_NEM\scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqgchal2\Documents\pypsa\results\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9987ED6-189B-4DF3-8906-D894413102EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C903724-A884-4F70-90EE-5A6FA5740457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{77D5C98B-CAFF-4229-8ED5-BA5A9CE7F873}"/>
+    <workbookView xWindow="-41388" yWindow="-2088" windowWidth="41496" windowHeight="16776" xr2:uid="{77D5C98B-CAFF-4229-8ED5-BA5A9CE7F873}"/>
   </bookViews>
   <sheets>
     <sheet name="scenarios_summary_20250709_1140" sheetId="1" r:id="rId1"/>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="82">
   <si>
     <t>Scenario</t>
   </si>
@@ -665,9 +665,6 @@
 VIC1-Solar: x6.0
 VIC1-Wind: x6.0
 VIC1-Battery: x6.0</t>
-  </si>
-  <si>
-    <t>8.2.1_6xVreCurtailReview</t>
   </si>
   <si>
     <t>% Gas increase on baseline</t>
@@ -961,17 +958,167 @@
 VIC1: 5.642</t>
   </si>
   <si>
-    <t>8.2.1_6xVreCurtailReview_5%</t>
-  </si>
-  <si>
-    <t>8.2.1_6xVreCurtailReview_10%</t>
+    <r>
+      <t>NSW1-Black Coal: x0.0
+NSW1-Gas: x0.5
+NSW1-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Rooftop Solar: x3.0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+NSW1-Solar: x3.0
+NSW1-Wind: x6.0
+NSW1-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Battery: x8.0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+QLD1-Black Coal: x0.0
+QLD1-Gas: x0.5
+QLD1-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Rooftop Solar: x3.0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+QLD1-Solar: x3.0
+QLD1-Wind: x6.0
+QLD1-Battery: x6.0
+SA1-Gas: x0.5
+SA1-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Rooftop Solar: x2.0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+SA1-Solar: x3.0
+SA1-Wind: x2.0
+SA1-Battery: x6.0
+TAS1-Gas: x0.5
+TAS1-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Rooftop Solar: x3.0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+TAS1-Wind: x5.0
+TAS1-Battery: x8.0
+VIC1-Gas: x0.5
+VIC1-Brown Coal: x0.0
+VIC1-Rooftop Solar: x4.0
+VIC1-Solar: x4.0
+VIC1-Wind: x4.0
+VIC1-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Battery: x8.0</t>
+    </r>
+  </si>
+  <si>
+    <t>8.3_VreCurtailReview</t>
+  </si>
+  <si>
+    <t>8.3_VreCurtailReview_5%</t>
+  </si>
+  <si>
+    <t>8.3_VreCurtailReview_10%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1139,6 +1286,14 @@
       <color rgb="FFABB2BF"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="36">
@@ -1777,13 +1932,13 @@
                   <c:v>8.2_6xVre&amp;BatteryZeroCoal</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8.2.1_6xVreCurtailReview</c:v>
+                  <c:v>8.3_VreCurtailReview</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>8.2.1_6xVreCurtailReview_5%</c:v>
+                  <c:v>8.3_VreCurtailReview_5%</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>8.2.1_6xVreCurtailReview_10%</c:v>
+                  <c:v>8.3_VreCurtailReview_10%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3017,25 +3172,25 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="21.42578125" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.5703125" customWidth="1"/>
-    <col min="8" max="8" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7265625" customWidth="1"/>
+    <col min="3" max="3" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="21.453125" customWidth="1"/>
+    <col min="6" max="6" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.54296875" customWidth="1"/>
+    <col min="8" max="8" width="29.1796875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3046,22 +3201,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>5</v>
@@ -3070,7 +3225,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="228.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="228.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -3090,7 +3245,7 @@
         <v>12.101000000000001</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H2" s="3">
         <v>1358.721</v>
@@ -3102,10 +3257,10 @@
         <v>0</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="252.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="252.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -3127,7 +3282,7 @@
         <v>18.152000000000001</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H3" s="3">
         <v>2570.9920000000002</v>
@@ -3140,10 +3295,10 @@
         <v>0</v>
       </c>
       <c r="K3" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="252.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="252.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -3165,7 +3320,7 @@
         <v>24.202000000000002</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H4" s="3">
         <v>1475.3119999999999</v>
@@ -3178,10 +3333,10 @@
         <v>0</v>
       </c>
       <c r="K4" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="252.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="252.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -3203,7 +3358,7 @@
         <v>48.404000000000003</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H5" s="3">
         <v>4.915</v>
@@ -3216,10 +3371,10 @@
         <v>0</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="312.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="312.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
@@ -3241,7 +3396,7 @@
         <v>48.404000000000003</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H6" s="3">
         <v>4.3079999999999998</v>
@@ -3254,10 +3409,10 @@
         <v>7.2779999999999996</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="312.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="312.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
@@ -3279,7 +3434,7 @@
         <v>55.103000000000002</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H7" s="3">
         <v>0.25700000000000001</v>
@@ -3292,10 +3447,10 @@
         <v>0</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="312.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="312.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
@@ -3317,7 +3472,7 @@
         <v>61.802</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H8" s="3">
         <v>0</v>
@@ -3330,10 +3485,10 @@
         <v>0</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="312.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="312.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
@@ -3355,7 +3510,7 @@
         <v>48.404000000000003</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H9" s="3">
         <v>3.403</v>
@@ -3368,10 +3523,10 @@
         <v>213.79400000000001</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="312.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="312.5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
@@ -3393,7 +3548,7 @@
         <v>48.404000000000003</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H10" s="3">
         <v>2.0910000000000002</v>
@@ -3406,10 +3561,10 @@
         <v>1732.2570000000001</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="252.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="252.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>25</v>
       </c>
@@ -3431,7 +3586,7 @@
         <v>48.404000000000003</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H11" s="3">
         <v>89569.538</v>
@@ -3444,10 +3599,10 @@
         <v>0</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="252.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="252.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>27</v>
       </c>
@@ -3469,7 +3624,7 @@
         <v>48.404000000000003</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H12" s="3">
         <v>140836.11300000001</v>
@@ -3482,10 +3637,10 @@
         <v>0</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="252.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="252.5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>29</v>
       </c>
@@ -3507,7 +3662,7 @@
         <v>48.404000000000003</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H13" s="3">
         <v>196435.91</v>
@@ -3520,10 +3675,10 @@
         <v>0</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="312.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="312.5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>31</v>
       </c>
@@ -3545,7 +3700,7 @@
         <v>48.404000000000003</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H14" s="3">
         <v>196304.30100000001</v>
@@ -3558,10 +3713,10 @@
         <v>0</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="312.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="312.5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>33</v>
       </c>
@@ -3583,7 +3738,7 @@
         <v>48.404000000000003</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H15" s="3">
         <v>196106.73</v>
@@ -3596,10 +3751,10 @@
         <v>9.3510000000000009</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="312.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="312.5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
@@ -3621,7 +3776,7 @@
         <v>48.404000000000003</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H16" s="3">
         <v>195782.60800000001</v>
@@ -3634,10 +3789,10 @@
         <v>91.778999999999996</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="312.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="312.5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>37</v>
       </c>
@@ -3659,7 +3814,7 @@
         <v>48.404000000000003</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H17" s="3">
         <v>246789.981</v>
@@ -3672,10 +3827,10 @@
         <v>86.075000000000003</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="312.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="312.5" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>39</v>
       </c>
@@ -3697,7 +3852,7 @@
         <v>72.605999999999995</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H18" s="3">
         <v>272944.29499999998</v>
@@ -3710,10 +3865,10 @@
         <v>0</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="312.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="312.5" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>41</v>
       </c>
@@ -3735,7 +3890,7 @@
         <v>72.605999999999995</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H19" s="3">
         <v>272625.527</v>
@@ -3748,10 +3903,10 @@
         <v>0</v>
       </c>
       <c r="K19" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="312.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="312.5" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>43</v>
       </c>
@@ -3773,7 +3928,7 @@
         <v>72.605999999999995</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H20" s="3">
         <v>272309.62</v>
@@ -3786,15 +3941,15 @@
         <v>8.5589999999999993</v>
       </c>
       <c r="K20" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="324.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="324.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="C21" s="3">
         <v>1868.6420000000001</v>
@@ -3811,7 +3966,7 @@
         <v>87.203999999999994</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H21" s="3">
         <v>80580.906000000003</v>
@@ -3824,15 +3979,15 @@
         <v>0</v>
       </c>
       <c r="K21" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="324.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="324.5" x14ac:dyDescent="0.35">
       <c r="A22" s="17" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" s="3">
         <v>2392.1559999999999</v>
@@ -3849,7 +4004,7 @@
         <v>87.203999999999994</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H22" s="3">
         <v>75486.803</v>
@@ -3862,15 +4017,15 @@
         <v>20.83</v>
       </c>
       <c r="K22" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="324.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="324.5" x14ac:dyDescent="0.35">
       <c r="A23" s="18" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" s="3">
         <v>3007.3119999999999</v>
@@ -3887,7 +4042,7 @@
         <v>87.203999999999994</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H23" s="3">
         <v>70496.773000000001</v>
@@ -3900,10 +4055,10 @@
         <v>74.921000000000006</v>
       </c>
       <c r="K23" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="I24" s="13"/>
     </row>
   </sheetData>
@@ -3922,7 +4077,7 @@
       <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Update conclusion and scenario summary .xlsx
</commit_message>
<xml_diff>
--- a/results/scenarios/scenarios_summary_gurobi_20250711_1007.xlsx
+++ b/results/scenarios/scenarios_summary_gurobi_20250711_1007.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqgchal2\Documents\pypsa\results\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C903724-A884-4F70-90EE-5A6FA5740457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F7D5A8-97D8-433D-9B77-DE10A7AB5C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-41388" yWindow="-2088" windowWidth="41496" windowHeight="16776" xr2:uid="{77D5C98B-CAFF-4229-8ED5-BA5A9CE7F873}"/>
   </bookViews>
@@ -668,9 +668,6 @@
   </si>
   <si>
     <t>% Gas increase on baseline</t>
-  </si>
-  <si>
-    <t>% Gas increase/decrease on 2024-25 (10,919MW)</t>
   </si>
   <si>
     <t>% increase on baseline</t>
@@ -1112,6 +1109,9 @@
   </si>
   <si>
     <t>8.3_VreCurtailReview_10%</t>
+  </si>
+  <si>
+    <t>% Gas increase/decrease on 2024-25 (10,919 GWh)</t>
   </si>
 </sst>
 </file>
@@ -1797,7 +1797,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>% Gas increase/decrease on 2024-25 (10,919MW)</c:v>
+                  <c:v>% Gas increase/decrease on 2024-25 (10,919 GWh)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3172,8 +3172,8 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3204,19 +3204,19 @@
         <v>45</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>46</v>
+        <v>81</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>5</v>
@@ -3245,7 +3245,7 @@
         <v>12.101000000000001</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H2" s="3">
         <v>1358.721</v>
@@ -3257,7 +3257,7 @@
         <v>0</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="252.5" x14ac:dyDescent="0.35">
@@ -3282,7 +3282,7 @@
         <v>18.152000000000001</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H3" s="3">
         <v>2570.9920000000002</v>
@@ -3295,7 +3295,7 @@
         <v>0</v>
       </c>
       <c r="K3" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="252.5" x14ac:dyDescent="0.35">
@@ -3320,7 +3320,7 @@
         <v>24.202000000000002</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H4" s="3">
         <v>1475.3119999999999</v>
@@ -3333,7 +3333,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="252.5" x14ac:dyDescent="0.35">
@@ -3358,7 +3358,7 @@
         <v>48.404000000000003</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H5" s="3">
         <v>4.915</v>
@@ -3371,7 +3371,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="312.5" x14ac:dyDescent="0.35">
@@ -3396,7 +3396,7 @@
         <v>48.404000000000003</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H6" s="3">
         <v>4.3079999999999998</v>
@@ -3409,7 +3409,7 @@
         <v>7.2779999999999996</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="312.5" x14ac:dyDescent="0.35">
@@ -3434,7 +3434,7 @@
         <v>55.103000000000002</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H7" s="3">
         <v>0.25700000000000001</v>
@@ -3447,7 +3447,7 @@
         <v>0</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="312.5" x14ac:dyDescent="0.35">
@@ -3472,7 +3472,7 @@
         <v>61.802</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H8" s="3">
         <v>0</v>
@@ -3485,7 +3485,7 @@
         <v>0</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="312.5" x14ac:dyDescent="0.35">
@@ -3510,7 +3510,7 @@
         <v>48.404000000000003</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H9" s="3">
         <v>3.403</v>
@@ -3523,7 +3523,7 @@
         <v>213.79400000000001</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="312.5" x14ac:dyDescent="0.35">
@@ -3548,7 +3548,7 @@
         <v>48.404000000000003</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H10" s="3">
         <v>2.0910000000000002</v>
@@ -3561,7 +3561,7 @@
         <v>1732.2570000000001</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="252.5" x14ac:dyDescent="0.35">
@@ -3586,7 +3586,7 @@
         <v>48.404000000000003</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H11" s="3">
         <v>89569.538</v>
@@ -3599,7 +3599,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="252.5" x14ac:dyDescent="0.35">
@@ -3624,7 +3624,7 @@
         <v>48.404000000000003</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H12" s="3">
         <v>140836.11300000001</v>
@@ -3637,7 +3637,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="252.5" x14ac:dyDescent="0.35">
@@ -3662,7 +3662,7 @@
         <v>48.404000000000003</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H13" s="3">
         <v>196435.91</v>
@@ -3675,7 +3675,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="312.5" x14ac:dyDescent="0.35">
@@ -3700,7 +3700,7 @@
         <v>48.404000000000003</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H14" s="3">
         <v>196304.30100000001</v>
@@ -3713,7 +3713,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="312.5" x14ac:dyDescent="0.35">
@@ -3738,7 +3738,7 @@
         <v>48.404000000000003</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H15" s="3">
         <v>196106.73</v>
@@ -3751,7 +3751,7 @@
         <v>9.3510000000000009</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="312.5" x14ac:dyDescent="0.35">
@@ -3776,7 +3776,7 @@
         <v>48.404000000000003</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H16" s="3">
         <v>195782.60800000001</v>
@@ -3789,7 +3789,7 @@
         <v>91.778999999999996</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="312.5" x14ac:dyDescent="0.35">
@@ -3814,7 +3814,7 @@
         <v>48.404000000000003</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H17" s="3">
         <v>246789.981</v>
@@ -3827,7 +3827,7 @@
         <v>86.075000000000003</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="312.5" x14ac:dyDescent="0.35">
@@ -3852,7 +3852,7 @@
         <v>72.605999999999995</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H18" s="3">
         <v>272944.29499999998</v>
@@ -3865,7 +3865,7 @@
         <v>0</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="312.5" x14ac:dyDescent="0.35">
@@ -3890,7 +3890,7 @@
         <v>72.605999999999995</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H19" s="3">
         <v>272625.527</v>
@@ -3903,7 +3903,7 @@
         <v>0</v>
       </c>
       <c r="K19" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="312.5" x14ac:dyDescent="0.35">
@@ -3928,7 +3928,7 @@
         <v>72.605999999999995</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H20" s="3">
         <v>272309.62</v>
@@ -3941,15 +3941,15 @@
         <v>8.5589999999999993</v>
       </c>
       <c r="K20" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="324.5" x14ac:dyDescent="0.35">
       <c r="A21" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C21" s="3">
         <v>1868.6420000000001</v>
@@ -3966,7 +3966,7 @@
         <v>87.203999999999994</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H21" s="3">
         <v>80580.906000000003</v>
@@ -3979,15 +3979,15 @@
         <v>0</v>
       </c>
       <c r="K21" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="324.5" x14ac:dyDescent="0.35">
       <c r="A22" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" s="3">
         <v>2392.1559999999999</v>
@@ -4004,7 +4004,7 @@
         <v>87.203999999999994</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H22" s="3">
         <v>75486.803</v>
@@ -4017,15 +4017,15 @@
         <v>20.83</v>
       </c>
       <c r="K22" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="324.5" x14ac:dyDescent="0.35">
       <c r="A23" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C23" s="3">
         <v>3007.3119999999999</v>
@@ -4042,7 +4042,7 @@
         <v>87.203999999999994</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H23" s="3">
         <v>70496.773000000001</v>
@@ -4055,7 +4055,7 @@
         <v>74.921000000000006</v>
       </c>
       <c r="K23" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">

</xml_diff>